<commit_message>
working sn and mn
</commit_message>
<xml_diff>
--- a/nvme_health_report.xlsx
+++ b/nvme_health_report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,30 +434,40 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Serial Number</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Model Number</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Percentage Used</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Temperature</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Critical Warning</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Available Spare</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Data Units Written</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Data Units Read</t>
         </is>
@@ -466,166 +476,50 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-08-14 14:41:13</t>
+          <t>2024-08-15 10:48:45</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>/dev/nvme0n1</t>
+          <t>/dev/nvme1n1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>PHCP416600301P9AGN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> SOLIDIGM SB5PH27E016T                   </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1911108498 (978.49 TB)</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>526519241 (269.58 TB)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-08-14 14:41:13</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>/dev/nvme0n2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1911108498 (978.49 TB)</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>526519241 (269.58 TB)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-08-14 14:41:13</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>/dev/nvme0n3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1911108498 (978.49 TB)</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>526519241 (269.58 TB)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-08-14 14:41:13</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>/dev/nvme1n1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>0 (0.00 B)</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>15 (7.68 MB)</t>
         </is>

</xml_diff>